<commit_message>
Add CV auto-build infrastructure: workflow, CSS, tests, and HTML link update
- Add GitHub Actions workflow (.github/workflows/build-cv.yml) to auto-build
  CV PDF and HTML from LaTeX source on push to main
- Add CSS stylesheet (css/cv.css) with @font-face for Dartmouth Ruzicka font,
  responsive design, and print styles
- Add comprehensive test suite (tests/test_build_cv.py) with 61 real tests
  covering LaTeX conversion, HTML generation, and PDF compilation
- Update people.html CV link to point to HTML version instead of PDF
- Regenerate CV PDF with latest content

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/people.xlsx
+++ b/data/people.xlsx
@@ -478,7 +478,6 @@
           <t>jeremy manning</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>lab director</t>
@@ -491,7 +490,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[&lt;a href="documents/JRM_CV.pdf" target="_blank"&gt;CV&lt;/a&gt;] [&lt;a href="https://scholar.google.com/citations?user=hskTzvcAAAAJ&amp;amp;hl=en" target="_blank"&gt;Google Scholar&lt;/a&gt;]</t>
+          <t>[&lt;a href="documents/JRM_CV.html" target="_blank"&gt;CV&lt;/a&gt;] [&lt;a href="https://scholar.google.com/citations?user=hskTzvcAAAAJ&amp;amp;hl=en" target="_blank"&gt;Google Scholar&lt;/a&gt;]</t>
         </is>
       </c>
     </row>
@@ -580,7 +579,6 @@
           <t>Paxton graduated from Dartmouth in 2019 with a BA in neuroscience and is continuing his research in the lab while applying to grad school. He's interested in creating new experiments and software tools to study classroom learning and model how memories change over time. Outside the lab, Paxton enjoys hiking, renovating old houses, and teaching Python.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -593,7 +591,6 @@
           <t>xinming xu</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>grad student</t>
@@ -604,7 +601,6 @@
           <t>Xinming's research uses memory retrieval paradigms to probe how narrative and real-life events are transformed into memory. He has a particular interest in memory for temporal structure. His outside-of-the-lab interests include exploring narratives, frisbee, and squash.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -617,7 +613,6 @@
           <t>aaryan agrawal</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -628,7 +623,6 @@
           <t>Aaryan is majoring in systems engineering and physics. He also takes courses in design, data science, and economics. Aaryan loves working out, slow meals, and playing games with his friends. He is an avid traveler and enjoys chasing new food and sights.</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -641,7 +635,6 @@
           <t>daniel carstensen</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -652,7 +645,6 @@
           <t>Daniel is a member of the class of 2024 from Munich, Germany and intends to major in mathematical data science and Japanese culture and language. His research interests revolve around the intersection of neuroscience and machine learning. Outside of lab work, he enjoys photography, reading, and skiing.</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -665,7 +657,6 @@
           <t>mira chiruvolu</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -676,7 +667,6 @@
           <t>Mira is a member of the class of 2025 studying cognitive science and creative writing. She is from the Bay Area, CA and outside of the lab she loves to write poetry, play basketball, and watch movies.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -689,7 +679,6 @@
           <t>kunal jha</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -700,7 +689,6 @@
           <t>Kunal is a member of the class of 2024, majoring in computer science and philosophy. His research interests lie at the intersection of machine learning and cognitive science, and he enjoys thinking about multi-agent systems. Outside of the lab, he spends most of his time training MMA, drumming, or playing video games.</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -713,7 +701,6 @@
           <t>wendy liang</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -724,7 +711,6 @@
           <t>Wendy is a member of the class of 2025 from Shenzhen, China and is double majoring in mathematical data science and economics. She enjoys sports, the outdoors, and would be very happy to chat about puzzles, board games, and problem-solving.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -737,7 +723,6 @@
           <t>jake mcdermid</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -748,7 +733,6 @@
           <t>Jake is a member of the class of 2025 from England, majoring in neuroscience. Outside of the lab, he enjoys watching sports, skiing, and spending time with friends outdoors.</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -761,7 +745,6 @@
           <t>ansh patel</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -772,7 +755,6 @@
           <t>Ansh is a member of the class of 2024 from Grafton, MA. He is studying mathematics and computer science to better explore his interests in finance and data science. Outside of the lab, he enjoys New England sports, traveling, and watching movies.</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -785,7 +767,6 @@
           <t>emma reeder</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -796,7 +777,6 @@
           <t>Emma is a member of the class of 2025, studying psychology and neuroscience. Outside of school, she enjoys skiing, reading, and making coffee.</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -809,7 +789,6 @@
           <t>om shah</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -820,7 +799,6 @@
           <t>Om is a member of the class of 2026 from Morganton, NC. He is on the pre-med track, and has many different interests ranging from biology to computer science.</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -833,7 +811,6 @@
           <t>zack somma</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>undergrad</t>
@@ -844,7 +821,6 @@
           <t>Zack is a member of the class of 2025 from New Hampshire, who plans on pursuing a double major in neuroscience and biomedical engineering sciences while on the pre-health track. In his free time, he plays hockey and tennis, enjoys spending time outdoors, and likes to explore various finance topics.</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -906,7 +882,6 @@
           <t>Gina Notaro</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>2017-2018</t>
@@ -1064,14 +1039,11 @@
           <t>Mark Taylor</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>QBS Masters Student 2021</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1079,14 +1051,11 @@
           <t>Max Bluestone</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>QBS Masters Student 2018-2019</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1094,7 +1063,6 @@
           <t>Tom Hao Chang</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>CS Masters Student 2016-2017</t>
@@ -1117,14 +1085,11 @@
           <t>Hanli Li</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>CS Masters Student 2016</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1213,7 +1178,6 @@
           <t>Emily Whitaker</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>2017-2018</t>

</xml_diff>

<commit_message>
added placeholder image, added new lab member info, updated cv, added some new lab member photos
</commit_message>
<xml_diff>
--- a/data/people.xlsx
+++ b/data/people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanning/contextlab.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A953CF9-3558-FD4D-BCCD-1C2E4C6B6836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C8CBD-2B8F-D340-9E8B-935520CB4A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="director" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="220">
   <si>
     <t>image</t>
   </si>
@@ -61,12 +61,69 @@
     <t>CV:documents/JRM_CV.html, "Google Scholar":https://scholar.google.com/citations?user=hskTzvcAAAAJ&amp;amp;hl=en</t>
   </si>
   <si>
+    <t>paxton_fitzpatrick.png</t>
+  </si>
+  <si>
+    <t>paxton fitzpatrick</t>
+  </si>
+  <si>
+    <t>http://paxtonfitzpatrick.github.io/</t>
+  </si>
+  <si>
+    <t>grad student</t>
+  </si>
+  <si>
+    <t>Paxton graduated from Dartmouth in 2019 with a BA in neuroscience and is continuing his research in the lab while applying to grad school. He's interested in creating new experiments and software tools to study classroom learning and model how memories change over time. Outside the lab, Paxton enjoys hiking, renovating old houses, and teaching Python.</t>
+  </si>
+  <si>
+    <t>xinming_xu.png</t>
+  </si>
+  <si>
+    <t>xinming xu</t>
+  </si>
+  <si>
+    <t>Xinming's research uses memory retrieval paradigms to probe how narrative and real-life events are transformed into memory. He has a particular interest in memory for temporal structure. His outside-of-the-lab interests include exploring narratives, frisbee, and squash.</t>
+  </si>
+  <si>
+    <t>claudia_gonciulea.jpeg</t>
+  </si>
+  <si>
+    <t>claudia gonciulea</t>
+  </si>
+  <si>
+    <t>https://contralto.github.io/</t>
+  </si>
+  <si>
+    <t>Claudia received her cognitive science and computer science degrees from the University of Michigan in 2023, and then studied learning and memory as a research specialist in the Penn Computational Cognitive Neuroscience lab. She’s interested in studying the factors that shape how new memories are created as we learn, and the subsequent changes to old memories that emerge as we experience the world. In addition to researching learning and memory, she loves going to museums, playing video and board games, baking, and being in nature.</t>
+  </si>
+  <si>
+    <t>jennifer xu</t>
+  </si>
+  <si>
+    <t>undergrad</t>
+  </si>
+  <si>
+    <t>om_shah.png</t>
+  </si>
+  <si>
+    <t>om shah</t>
+  </si>
+  <si>
+    <t>Om is a member of the class of 2026 from Morganton, NC. He is on the pre-med track, and has many different interests ranging from biology to computer science.</t>
+  </si>
+  <si>
+    <t>sarah parigela</t>
+  </si>
+  <si>
+    <t>chelsea joe</t>
+  </si>
+  <si>
+    <t>jacob bacus</t>
+  </si>
+  <si>
     <t>aidan miller</t>
   </si>
   <si>
-    <t>undergrad</t>
-  </si>
-  <si>
     <t>alexandra wingo</t>
   </si>
   <si>
@@ -88,24 +145,6 @@
     <t>ben hanson</t>
   </si>
   <si>
-    <t>chelsea joe</t>
-  </si>
-  <si>
-    <t>claudia_gonciulea.jpeg</t>
-  </si>
-  <si>
-    <t>claudia gonciulea</t>
-  </si>
-  <si>
-    <t>https://contralto.github.io/</t>
-  </si>
-  <si>
-    <t>grad student</t>
-  </si>
-  <si>
-    <t>Claudia received her cognitive science and computer science degrees from the University of Michigan in 2023, and then studied learning and memory as a research specialist in the Penn Computational Cognitive Neuroscience lab. She’s interested in studying the factors that shape how new memories are created as we learn, and the subsequent changes to old memories that emerge as we experience the world. In addition to researching learning and memory, she loves going to museums, playing video and board games, baking, and being in nature.</t>
-  </si>
-  <si>
     <t>ellie mattox</t>
   </si>
   <si>
@@ -118,12 +157,6 @@
     <t>jackson c. sandrich</t>
   </si>
   <si>
-    <t>jacob bacus</t>
-  </si>
-  <si>
-    <t>jennifer xu</t>
-  </si>
-  <si>
     <t>joy maina</t>
   </si>
   <si>
@@ -133,48 +166,15 @@
     <t>luca gandrud</t>
   </si>
   <si>
-    <t>om_shah.png</t>
-  </si>
-  <si>
-    <t>om shah</t>
-  </si>
-  <si>
-    <t>Om is a member of the class of 2026 from Morganton, NC. He is on the pre-med track, and has many different interests ranging from biology to computer science.</t>
-  </si>
-  <si>
     <t>owen phillips</t>
   </si>
   <si>
-    <t>paxton_fitzpatrick.png</t>
-  </si>
-  <si>
-    <t>paxton fitzpatrick</t>
-  </si>
-  <si>
-    <t>http://paxtonfitzpatrick.github.io/</t>
-  </si>
-  <si>
-    <t>Paxton graduated from Dartmouth in 2019 with a BA in neuroscience and is continuing his research in the lab while applying to grad school. He's interested in creating new experiments and software tools to study classroom learning and model how memories change over time. Outside the lab, Paxton enjoys hiking, renovating old houses, and teaching Python.</t>
-  </si>
-  <si>
     <t>sam haskel</t>
   </si>
   <si>
-    <t>sarah parigela</t>
-  </si>
-  <si>
     <t>will lehman</t>
   </si>
   <si>
-    <t>xinming_xu.png</t>
-  </si>
-  <si>
-    <t>xinming xu</t>
-  </si>
-  <si>
-    <t>Xinming's research uses memory retrieval paradigms to probe how narrative and real-life events are transformed into memory. He has a particular interest in memory for temporal structure. His outside-of-the-lab interests include exploring narratives, frisbee, and squash.</t>
-  </si>
-  <si>
     <t>years</t>
   </si>
   <si>
@@ -319,6 +319,12 @@
     <t>then a CDL grad student!</t>
   </si>
   <si>
+    <t>Jake McDermid</t>
+  </si>
+  <si>
+    <t>2023-2025</t>
+  </si>
+  <si>
     <t>Ameer Talha Yasser</t>
   </si>
   <si>
@@ -613,6 +619,15 @@
     <t>Rockmore Lab, Dartmouth College (Director: Dan Rockmore)</t>
   </si>
   <si>
+    <t>Vu Lab</t>
+  </si>
+  <si>
+    <t>https://faculty-directory.dartmouth.edu/tam-vu</t>
+  </si>
+  <si>
+    <t>Vu Lab, Dartmouth College (Director: Tam Vu)</t>
+  </si>
+  <si>
     <t>Nautiyal Lab</t>
   </si>
   <si>
@@ -640,26 +655,44 @@
     <t>Chameleon Studios (Director: Talia Manning)</t>
   </si>
   <si>
-    <t>Jake McDermid</t>
-  </si>
-  <si>
-    <t>2023-2025</t>
-  </si>
-  <si>
-    <t>Vu Lab</t>
-  </si>
-  <si>
-    <t>https://faculty-directory.dartmouth.edu/tam-vu</t>
-  </si>
-  <si>
-    <t>Vu Lab, Dartmouth College (Director: Tam Vu)</t>
+    <t>https://pbs.dartmouth.edu/people/jeremy-r-manning</t>
+  </si>
+  <si>
+    <t>Alishba is a visiting research assistant interested in the intersection of memory, narrative processing, and the mechanisms behind forgetting what to forget. She holds an undergraduate degree in Biology from LUMS and has previously worked on fMRI-based disease analysis. At the CDL, she is exploring how recall and prediction shape memory dynamics over time using naturalistic stimuli.</t>
+  </si>
+  <si>
+    <t>Andrew Richardson is a Mathematics and Economics double major from Minneapolis, MN. Outside of academics, he enjoys playing tennis and soccer.</t>
+  </si>
+  <si>
+    <t>Angelyn is a member of the class of 2028 from the Bay Area, CA, planning on majoring in cognitive science. In her free time, she enjoys singing, reading, puzzle games, and creative writing.</t>
+  </si>
+  <si>
+    <t>Annabelle Morrow is a member of the class of 2028 from Hong Kong. She is planning to major in economics and minor in human-centered design. Outside of class, she enjoys running and spending time outdoors.</t>
+  </si>
+  <si>
+    <t>Ben is a member of the class of 2027 studying PPE and human-centered design. Outside of school, he enjoy skiing, surfing, and coffee.</t>
+  </si>
+  <si>
+    <t>Ellie is a member of the class of 2027 from Austin, TX and is majoring in neuroscience with a minor in human-centered design. Outside of the lab she enjoys playing volleyball on Dartmouth's Varsity team, spending time outside, and hanging out with friends.</t>
+  </si>
+  <si>
+    <t>From Taipei and Boston, Kevin is a ‘29 studying Applied Math and CS. He is passionate about quantitative finance, machine learning, and health analytics. His long term goal is to develop data-driven solutions to optimize inefficiencies in the US healthcare system.</t>
+  </si>
+  <si>
+    <t>Owen is a ‘28 from Costa Mesa, California. He plans to major in Math and minor in Engineering and Computer Science. In his free time, he enjoys philatelics, post-hardcore music, fashion/art history, and logic puzzles.</t>
+  </si>
+  <si>
+    <t>Will is a '27 from Salt Lake City, Utah. He likes skiing, playing hockey, and working on new projects.</t>
+  </si>
+  <si>
+    <t>ben_hanson.HEIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,18 +701,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -690,12 +715,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -704,14 +744,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1018,53 +1058,54 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="5" max="5" width="52.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1077,293 +1118,390 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1374,82 +1512,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1462,117 +1590,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1583,82 +1692,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1671,521 +1770,512 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B3" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B8" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B11" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B16" t="s">
         <v>118</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B19" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>131</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>132</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>133</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>135</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B32" t="s">
         <v>136</v>
       </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="2" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>140</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B36" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B37" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>144</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="B38" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="B41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="B42" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B47" s="2" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="B48" t="s">
         <v>157</v>
       </c>
-      <c r="B50" s="2" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B51" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B53" s="2" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B54" s="2" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>166</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="B56" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>169</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="B58" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>170</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="B59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>171</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="B60" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>172</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>165</v>
+      <c r="B61" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2197,150 +2287,140 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="61.83203125" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="80" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C3" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B4" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C4" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C5" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" t="s">
         <v>189</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C6" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" t="s">
         <v>192</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C7" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>206</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" t="s">
         <v>207</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C12" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sort members by role/date, add profile borders, use placeholder default
- Sort members sheet by role (grad students first) then join date
- Add hand-drawn borders to profile photos: ben_hanson, ellie_mattox,
  andrew_richardson, claudia_gonciulea, placeholder
- Convert HEIC/JPEG photos to PNG format
- Update build_people.py to use placeholder.png for members without images
- Regenerate people.html with sorted members and placeholder defaults

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/people.xlsx
+++ b/data/people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanning/contextlab.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C8CBD-2B8F-D340-9E8B-935520CB4A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B2CFD7-5C6C-2E4F-96B8-39800594F45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14740" yWindow="11580" windowWidth="34560" windowHeight="21660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="director" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="230">
   <si>
     <t>image</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Xinming's research uses memory retrieval paradigms to probe how narrative and real-life events are transformed into memory. He has a particular interest in memory for temporal structure. His outside-of-the-lab interests include exploring narratives, frisbee, and squash.</t>
   </si>
   <si>
-    <t>claudia_gonciulea.jpeg</t>
-  </si>
-  <si>
     <t>claudia gonciulea</t>
   </si>
   <si>
@@ -148,18 +145,12 @@
     <t>ellie mattox</t>
   </si>
   <si>
-    <t>emmy thornton</t>
-  </si>
-  <si>
     <t>evan mcdermid</t>
   </si>
   <si>
     <t>jackson c. sandrich</t>
   </si>
   <si>
-    <t>joy maina</t>
-  </si>
-  <si>
     <t>kevin chang</t>
   </si>
   <si>
@@ -685,7 +676,46 @@
     <t>Will is a '27 from Salt Lake City, Utah. He likes skiing, playing hockey, and working on new projects.</t>
   </si>
   <si>
-    <t>ben_hanson.HEIC</t>
+    <t>ellie_mattox.png</t>
+  </si>
+  <si>
+    <t>ben_hanson.png</t>
+  </si>
+  <si>
+    <t>claudia_gonciulea.png</t>
+  </si>
+  <si>
+    <t>Jennifer is planning to double major in Quantitative Social Science and Comparative Literature. She has a background in mathematics and programming, and is interested in the humanities and literature. She hopes to use machine learning to enhance our understanding of humanitarian issues.</t>
+  </si>
+  <si>
+    <t>Sarah is interested in cognitive science, psychology, and neuroscience. She is working on using EEG to track how people learn from online course videos.</t>
+  </si>
+  <si>
+    <t>Chelsea is a Computer Science and Neuroscience double major. She is interested in artificial intelligence, machine learning, and building computational models.</t>
+  </si>
+  <si>
+    <t>Jacob's work is focused on using machine learning and deep learning models to understand mental health. He is also interested in how cognitive and mental function relate to one another.</t>
+  </si>
+  <si>
+    <t>Aidan is a pre-med student interested in how we can learn as quickly and efficiently as possible. He is a dedicated practitioner of memory "hacks" like the chaine method, story method, and method of loci.</t>
+  </si>
+  <si>
+    <t>Alexandra is interested in education technology and brings to the lab her extensive computer science experience. She is especially interested in helping students with learning differences, and in developing brain-based learning tools.</t>
+  </si>
+  <si>
+    <t>Azaire is a Mathematics and Anthropology double major. She is particularly interested in understanding complex systems like brain networks and financial markets.</t>
+  </si>
+  <si>
+    <t>Evan is a Mathematics major and Computer Science minor. He is interested in algorithmic trading, algorithmic problem solving, and building models of financial market dynamics.</t>
+  </si>
+  <si>
+    <t>Jax is a Mathematics and Economics double major. He is interested in using EEG to understand how people learn new concepts and skills.</t>
+  </si>
+  <si>
+    <t>Luca is a Neuroscience major who is passionate about how we can use technology and neuroscience to enhance learning in everyday life. He is also interested in wearable brain recording devices.</t>
+  </si>
+  <si>
+    <t>Sam is a Quantitative Social Science and Economics double major. He is interested in how social peer influences shape beliefs and affect how people make decisions.</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1127,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1116,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1187,321 +1217,321 @@
     </row>
     <row r="4" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>219</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>223</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>225</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>216</v>
+      </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1524,61 +1554,61 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1602,85 +1632,85 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1704,61 +1734,61 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1779,503 +1809,503 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2296,131 +2326,131 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
         <v>177</v>
       </c>
-      <c r="B3" t="s">
-        <v>180</v>
-      </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Jacob Bacus photo and bio
- Add bordered profile photo for Jacob Bacus
- Add bio: CS and Middle Eastern Studies, class of 2027,
  ML/deep learning for mental health research
- Regenerate people.html

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/people.xlsx
+++ b/data/people.xlsx
@@ -719,7 +719,11 @@
       <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>jacob_bacus.png</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>jacob bacus</t>
@@ -733,7 +737,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Jacob's work is focused on using machine learning and deep learning models to understand mental health. He is also interested in how cognitive and mental function relate to one another.</t>
+          <t>Jacob is a member of the class of 2027 from Kansas City, Missouri studying Computer Science and Middle Eastern Studies. Jacob's work in the lab focuses on using machine learning and deep learning models to understand mental health. He is also interested in how cognitive and mental function relate to one another.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>

</xml_diff>